<commit_message>
JWSTSIAF266 May 2023 NIRSpec pysiaf update, siaf positions of NRS IFU aperture have changed and been updated.
</commit_message>
<xml_diff>
--- a/pysiaf/pre_delivery_data/NIRSpec/NIRSpec_SIAF.xlsx
+++ b/pysiaf/pre_delivery_data/NIRSpec/NIRSpec_SIAF.xlsx
@@ -6703,17 +6703,17 @@
       </c>
       <c r="P12" s="3" t="inlineStr">
         <is>
-          <t>299.8354797363281</t>
+          <t>300.00927734375</t>
         </is>
       </c>
       <c r="Q12" s="3" t="inlineStr">
         <is>
-          <t>-498.2568054199219</t>
+          <t>-498.0792541503906</t>
         </is>
       </c>
       <c r="R12" s="3" t="inlineStr">
         <is>
-          <t>138.9725341796875</t>
+          <t>138.97164916992188</t>
         </is>
       </c>
       <c r="S12" s="3" t="inlineStr">
@@ -6743,42 +6743,42 @@
       </c>
       <c r="X12" s="3" t="inlineStr">
         <is>
-          <t>1.4861502647399902</t>
+          <t>1.4861249923706055</t>
         </is>
       </c>
       <c r="Y12" s="3" t="inlineStr">
         <is>
-          <t>1.4858390092849731</t>
+          <t>1.4858232736587524</t>
         </is>
       </c>
       <c r="Z12" s="3" t="inlineStr">
         <is>
-          <t>-1.6110278367996216</t>
+          <t>-1.61100435256958</t>
         </is>
       </c>
       <c r="AA12" s="3" t="inlineStr">
         <is>
-          <t>-1.6113126277923584</t>
+          <t>-1.6112955808639526</t>
         </is>
       </c>
       <c r="AB12" s="3" t="inlineStr">
         <is>
-          <t>1.6356580257415771</t>
+          <t>1.6356810331344604</t>
         </is>
       </c>
       <c r="AC12" s="3" t="inlineStr">
         <is>
-          <t>-1.5640443563461304</t>
+          <t>-1.56397545337677</t>
         </is>
       </c>
       <c r="AD12" s="3" t="inlineStr">
         <is>
-          <t>-1.526963472366333</t>
+          <t>-1.5269883871078491</t>
         </is>
       </c>
       <c r="AE12" s="3" t="inlineStr">
         <is>
-          <t>1.6731914281845093</t>
+          <t>1.6731635332107544</t>
         </is>
       </c>
       <c r="AF12" s="3" t="inlineStr">
@@ -7295,17 +7295,17 @@
       </c>
       <c r="P13" s="3" t="inlineStr">
         <is>
-          <t>299.7933654785156</t>
+          <t>299.9671630859375</t>
         </is>
       </c>
       <c r="Q13" s="3" t="inlineStr">
         <is>
-          <t>-498.365966796875</t>
+          <t>-498.1883850097656</t>
         </is>
       </c>
       <c r="R13" s="3" t="inlineStr">
         <is>
-          <t>138.97267150878906</t>
+          <t>138.97178649902344</t>
         </is>
       </c>
       <c r="S13" s="3" t="inlineStr">
@@ -7335,42 +7335,42 @@
       </c>
       <c r="X13" s="3" t="inlineStr">
         <is>
-          <t>0.048907458782196045</t>
+          <t>0.04886263608932495</t>
         </is>
       </c>
       <c r="Y13" s="3" t="inlineStr">
         <is>
-          <t>0.048874735832214355</t>
+          <t>0.04885953664779663</t>
         </is>
       </c>
       <c r="Z13" s="3" t="inlineStr">
         <is>
-          <t>-0.05452162027359009</t>
+          <t>-0.05455988645553589</t>
         </is>
       </c>
       <c r="AA13" s="3" t="inlineStr">
         <is>
-          <t>-0.05455499887466431</t>
+          <t>-0.054556846618652344</t>
         </is>
       </c>
       <c r="AB13" s="3" t="inlineStr">
         <is>
-          <t>1.602219820022583</t>
+          <t>1.6022435426712036</t>
         </is>
       </c>
       <c r="AC13" s="3" t="inlineStr">
         <is>
-          <t>-1.6030187606811523</t>
+          <t>-1.6029717922210693</t>
         </is>
       </c>
       <c r="AD13" s="3" t="inlineStr">
         <is>
-          <t>-1.6017649173736572</t>
+          <t>-1.6017398834228516</t>
         </is>
       </c>
       <c r="AE13" s="3" t="inlineStr">
         <is>
-          <t>1.6034563779830933</t>
+          <t>1.603475570678711</t>
         </is>
       </c>
       <c r="AF13" s="3" t="inlineStr">
@@ -7887,17 +7887,17 @@
       </c>
       <c r="P14" s="3" t="inlineStr">
         <is>
-          <t>299.8705749511719</t>
+          <t>300.04437255859375</t>
         </is>
       </c>
       <c r="Q14" s="3" t="inlineStr">
         <is>
-          <t>-498.297119140625</t>
+          <t>-498.11956787109375</t>
         </is>
       </c>
       <c r="R14" s="3" t="inlineStr">
         <is>
-          <t>138.97232055664062</t>
+          <t>138.971435546875</t>
         </is>
       </c>
       <c r="S14" s="3" t="inlineStr">
@@ -7927,42 +7927,42 @@
       </c>
       <c r="X14" s="3" t="inlineStr">
         <is>
-          <t>0.04878842830657959</t>
+          <t>0.04880702495574951</t>
         </is>
       </c>
       <c r="Y14" s="3" t="inlineStr">
         <is>
-          <t>0.048778533935546875</t>
+          <t>0.04878300428390503</t>
         </is>
       </c>
       <c r="Z14" s="3" t="inlineStr">
         <is>
-          <t>-0.054554760456085205</t>
+          <t>-0.054550349712371826</t>
         </is>
       </c>
       <c r="AA14" s="3" t="inlineStr">
         <is>
-          <t>-0.05454188585281372</t>
+          <t>-0.054566383361816406</t>
         </is>
       </c>
       <c r="AB14" s="3" t="inlineStr">
         <is>
-          <t>1.6022059917449951</t>
+          <t>1.602203607559204</t>
         </is>
       </c>
       <c r="AC14" s="3" t="inlineStr">
         <is>
-          <t>-1.6029894351959229</t>
+          <t>-1.6029655933380127</t>
         </is>
       </c>
       <c r="AD14" s="3" t="inlineStr">
         <is>
-          <t>-1.601762294769287</t>
+          <t>-1.6017401218414307</t>
         </is>
       </c>
       <c r="AE14" s="3" t="inlineStr">
         <is>
-          <t>1.6034760475158691</t>
+          <t>1.6034750938415527</t>
         </is>
       </c>
       <c r="AF14" s="3" t="inlineStr">
@@ -8479,17 +8479,17 @@
       </c>
       <c r="P15" s="3" t="inlineStr">
         <is>
-          <t>299.7160949707031</t>
+          <t>299.889892578125</t>
         </is>
       </c>
       <c r="Q15" s="3" t="inlineStr">
         <is>
-          <t>-498.4348449707031</t>
+          <t>-498.2572937011719</t>
         </is>
       </c>
       <c r="R15" s="3" t="inlineStr">
         <is>
-          <t>138.97303771972656</t>
+          <t>138.97215270996094</t>
         </is>
       </c>
       <c r="S15" s="3" t="inlineStr">
@@ -8519,42 +8519,42 @@
       </c>
       <c r="X15" s="3" t="inlineStr">
         <is>
-          <t>0.04896080493927002</t>
+          <t>0.048979103565216064</t>
         </is>
       </c>
       <c r="Y15" s="3" t="inlineStr">
         <is>
-          <t>0.04897361993789673</t>
+          <t>0.04895538091659546</t>
         </is>
       </c>
       <c r="Z15" s="3" t="inlineStr">
         <is>
-          <t>-0.05450892448425293</t>
+          <t>-0.0545041561126709</t>
         </is>
       </c>
       <c r="AA15" s="3" t="inlineStr">
         <is>
-          <t>-0.05452471971511841</t>
+          <t>-0.05450642108917236</t>
         </is>
       </c>
       <c r="AB15" s="3" t="inlineStr">
         <is>
-          <t>1.602216362953186</t>
+          <t>1.6022142171859741</t>
         </is>
       </c>
       <c r="AC15" s="3" t="inlineStr">
         <is>
-          <t>-1.603004813194275</t>
+          <t>-1.6030011177062988</t>
         </is>
       </c>
       <c r="AD15" s="3" t="inlineStr">
         <is>
-          <t>-1.601744532585144</t>
+          <t>-1.6017223596572876</t>
         </is>
       </c>
       <c r="AE15" s="3" t="inlineStr">
         <is>
-          <t>1.603433609008789</t>
+          <t>1.6034297943115234</t>
         </is>
       </c>
       <c r="AF15" s="3" t="inlineStr">
@@ -9071,17 +9071,17 @@
       </c>
       <c r="P16" s="3" t="inlineStr">
         <is>
-          <t>299.9477233886719</t>
+          <t>300.12152099609375</t>
         </is>
       </c>
       <c r="Q16" s="3" t="inlineStr">
         <is>
-          <t>-498.22833251953125</t>
+          <t>-498.05078125</t>
         </is>
       </c>
       <c r="R16" s="3" t="inlineStr">
         <is>
-          <t>138.9719696044922</t>
+          <t>138.97108459472656</t>
         </is>
       </c>
       <c r="S16" s="3" t="inlineStr">
@@ -9111,42 +9111,42 @@
       </c>
       <c r="X16" s="3" t="inlineStr">
         <is>
-          <t>0.04873281717300415</t>
+          <t>0.04870796203613281</t>
         </is>
       </c>
       <c r="Y16" s="3" t="inlineStr">
         <is>
-          <t>0.04870504140853882</t>
+          <t>0.04870980978012085</t>
         </is>
       </c>
       <c r="Z16" s="3" t="inlineStr">
         <is>
-          <t>-0.0545651912689209</t>
+          <t>-0.05456042289733887</t>
         </is>
       </c>
       <c r="AA16" s="3" t="inlineStr">
         <is>
-          <t>-0.054574549198150635</t>
+          <t>-0.05455636978149414</t>
         </is>
       </c>
       <c r="AB16" s="3" t="inlineStr">
         <is>
-          <t>1.6021661758422852</t>
+          <t>1.6021668910980225</t>
         </is>
       </c>
       <c r="AC16" s="3" t="inlineStr">
         <is>
-          <t>-1.6029400825500488</t>
+          <t>-1.6029162406921387</t>
         </is>
       </c>
       <c r="AD16" s="3" t="inlineStr">
         <is>
-          <t>-1.6017396450042725</t>
+          <t>-1.601717472076416</t>
         </is>
       </c>
       <c r="AE16" s="3" t="inlineStr">
         <is>
-          <t>1.6034557819366455</t>
+          <t>1.6034518480300903</t>
         </is>
       </c>
       <c r="AF16" s="3" t="inlineStr">
@@ -9663,17 +9663,17 @@
       </c>
       <c r="P17" s="3" t="inlineStr">
         <is>
-          <t>299.6387939453125</t>
+          <t>299.8125915527344</t>
         </is>
       </c>
       <c r="Q17" s="3" t="inlineStr">
         <is>
-          <t>-498.5037536621094</t>
+          <t>-498.3262023925781</t>
         </is>
       </c>
       <c r="R17" s="3" t="inlineStr">
         <is>
-          <t>138.973388671875</t>
+          <t>138.97250366210938</t>
         </is>
       </c>
       <c r="S17" s="3" t="inlineStr">
@@ -9703,42 +9703,42 @@
       </c>
       <c r="X17" s="3" t="inlineStr">
         <is>
-          <t>0.04903346300125122</t>
+          <t>0.04905205965042114</t>
         </is>
       </c>
       <c r="Y17" s="3" t="inlineStr">
         <is>
-          <t>0.049030184745788574</t>
+          <t>0.04903453588485718</t>
         </is>
       </c>
       <c r="Z17" s="3" t="inlineStr">
         <is>
-          <t>-0.05453544855117798</t>
+          <t>-0.054511070251464844</t>
         </is>
       </c>
       <c r="AA17" s="3" t="inlineStr">
         <is>
-          <t>-0.05451810359954834</t>
+          <t>-0.05452251434326172</t>
         </is>
       </c>
       <c r="AB17" s="3" t="inlineStr">
         <is>
-          <t>1.6021900177001953</t>
+          <t>1.6021878719329834</t>
         </is>
       </c>
       <c r="AC17" s="3" t="inlineStr">
         <is>
-          <t>-1.6029881238937378</t>
+          <t>-1.6029644012451172</t>
         </is>
       </c>
       <c r="AD17" s="3" t="inlineStr">
         <is>
-          <t>-1.6016781330108643</t>
+          <t>-1.6016790866851807</t>
         </is>
       </c>
       <c r="AE17" s="3" t="inlineStr">
         <is>
-          <t>1.6033909320831299</t>
+          <t>1.6033670902252197</t>
         </is>
       </c>
       <c r="AF17" s="3" t="inlineStr">
@@ -10255,17 +10255,17 @@
       </c>
       <c r="P18" s="3" t="inlineStr">
         <is>
-          <t>300.02484130859375</t>
+          <t>300.1986389160156</t>
         </is>
       </c>
       <c r="Q18" s="3" t="inlineStr">
         <is>
-          <t>-498.15960693359375</t>
+          <t>-497.9820556640625</t>
         </is>
       </c>
       <c r="R18" s="3" t="inlineStr">
         <is>
-          <t>138.9716033935547</t>
+          <t>138.97071838378906</t>
         </is>
       </c>
       <c r="S18" s="3" t="inlineStr">
@@ -10295,42 +10295,42 @@
       </c>
       <c r="X18" s="3" t="inlineStr">
         <is>
-          <t>0.048630475997924805</t>
+          <t>0.04862862825393677</t>
         </is>
       </c>
       <c r="Y18" s="3" t="inlineStr">
         <is>
-          <t>0.04863220453262329</t>
+          <t>0.04861396551132202</t>
         </is>
       </c>
       <c r="Z18" s="3" t="inlineStr">
         <is>
-          <t>-0.05457496643066406</t>
+          <t>-0.05457019805908203</t>
         </is>
       </c>
       <c r="AA18" s="3" t="inlineStr">
         <is>
-          <t>-0.05456775426864624</t>
+          <t>-0.05459260940551758</t>
         </is>
       </c>
       <c r="AB18" s="3" t="inlineStr">
         <is>
-          <t>1.6020863056182861</t>
+          <t>1.6021071672439575</t>
         </is>
       </c>
       <c r="AC18" s="3" t="inlineStr">
         <is>
-          <t>-1.6028907299041748</t>
+          <t>-1.6028869152069092</t>
         </is>
       </c>
       <c r="AD18" s="3" t="inlineStr">
         <is>
-          <t>-1.6017169952392578</t>
+          <t>-1.6016947031021118</t>
         </is>
       </c>
       <c r="AE18" s="3" t="inlineStr">
         <is>
-          <t>1.6033892631530762</t>
+          <t>1.6033883094787598</t>
         </is>
       </c>
       <c r="AF18" s="3" t="inlineStr">
@@ -10847,17 +10847,17 @@
       </c>
       <c r="P19" s="3" t="inlineStr">
         <is>
-          <t>299.5614318847656</t>
+          <t>299.7352294921875</t>
         </is>
       </c>
       <c r="Q19" s="3" t="inlineStr">
         <is>
-          <t>-498.5727233886719</t>
+          <t>-498.3951721191406</t>
         </is>
       </c>
       <c r="R19" s="3" t="inlineStr">
         <is>
-          <t>138.9737548828125</t>
+          <t>138.97286987304688</t>
         </is>
       </c>
       <c r="S19" s="3" t="inlineStr">
@@ -10887,42 +10887,42 @@
       </c>
       <c r="X19" s="3" t="inlineStr">
         <is>
-          <t>0.04912692308425903</t>
+          <t>0.049122512340545654</t>
         </is>
       </c>
       <c r="Y19" s="3" t="inlineStr">
         <is>
-          <t>0.04908883571624756</t>
+          <t>0.049113333225250244</t>
         </is>
       </c>
       <c r="Z19" s="3" t="inlineStr">
         <is>
-          <t>-0.05449676513671875</t>
+          <t>-0.054472386837005615</t>
         </is>
       </c>
       <c r="AA19" s="3" t="inlineStr">
         <is>
-          <t>-0.054513752460479736</t>
+          <t>-0.05449509620666504</t>
         </is>
       </c>
       <c r="AB19" s="3" t="inlineStr">
         <is>
-          <t>1.6021406650543213</t>
+          <t>1.6021184921264648</t>
         </is>
       </c>
       <c r="AC19" s="3" t="inlineStr">
         <is>
-          <t>-1.6029282808303833</t>
+          <t>-1.602927565574646</t>
         </is>
       </c>
       <c r="AD19" s="3" t="inlineStr">
         <is>
-          <t>-1.6015946865081787</t>
+          <t>-1.6015955209732056</t>
         </is>
       </c>
       <c r="AE19" s="3" t="inlineStr">
         <is>
-          <t>1.6033051013946533</t>
+          <t>1.6033012866973877</t>
         </is>
       </c>
       <c r="AF19" s="3" t="inlineStr">
@@ -11439,17 +11439,17 @@
       </c>
       <c r="P20" s="3" t="inlineStr">
         <is>
-          <t>300.10186767578125</t>
+          <t>300.2756652832031</t>
         </is>
       </c>
       <c r="Q20" s="3" t="inlineStr">
         <is>
-          <t>-498.0909118652344</t>
+          <t>-497.9133605957031</t>
         </is>
       </c>
       <c r="R20" s="3" t="inlineStr">
         <is>
-          <t>138.97125244140625</t>
+          <t>138.97036743164062</t>
         </is>
       </c>
       <c r="S20" s="3" t="inlineStr">
@@ -11479,42 +11479,42 @@
       </c>
       <c r="X20" s="3" t="inlineStr">
         <is>
-          <t>0.04855144023895264</t>
+          <t>0.0485265851020813</t>
         </is>
       </c>
       <c r="Y20" s="3" t="inlineStr">
         <is>
-          <t>0.048542022705078125</t>
+          <t>0.048523783683776855</t>
         </is>
       </c>
       <c r="Z20" s="3" t="inlineStr">
         <is>
-          <t>-0.05455905199050903</t>
+          <t>-0.05457723140716553</t>
         </is>
       </c>
       <c r="AA20" s="3" t="inlineStr">
         <is>
-          <t>-0.054580748081207275</t>
+          <t>-0.05458259582519531</t>
         </is>
       </c>
       <c r="AB20" s="3" t="inlineStr">
         <is>
-          <t>1.6020267009735107</t>
+          <t>1.602027416229248</t>
         </is>
       </c>
       <c r="AC20" s="3" t="inlineStr">
         <is>
-          <t>-1.6027753353118896</t>
+          <t>-1.602771520614624</t>
         </is>
       </c>
       <c r="AD20" s="3" t="inlineStr">
         <is>
-          <t>-1.6016311645507812</t>
+          <t>-1.6016290187835693</t>
         </is>
       </c>
       <c r="AE20" s="3" t="inlineStr">
         <is>
-          <t>1.6033458709716797</t>
+          <t>1.6033650636672974</t>
         </is>
       </c>
       <c r="AF20" s="3" t="inlineStr">
@@ -12031,17 +12031,17 @@
       </c>
       <c r="P21" s="3" t="inlineStr">
         <is>
-          <t>299.4840087890625</t>
+          <t>299.6578369140625</t>
         </is>
       </c>
       <c r="Q21" s="3" t="inlineStr">
         <is>
-          <t>-498.6417541503906</t>
+          <t>-498.46417236328125</t>
         </is>
       </c>
       <c r="R21" s="3" t="inlineStr">
         <is>
-          <t>138.97410583496094</t>
+          <t>138.9732208251953</t>
         </is>
       </c>
       <c r="S21" s="3" t="inlineStr">
@@ -12071,42 +12071,42 @@
       </c>
       <c r="X21" s="3" t="inlineStr">
         <is>
-          <t>0.04921692609786987</t>
+          <t>0.049192190170288086</t>
         </is>
       </c>
       <c r="Y21" s="3" t="inlineStr">
         <is>
-          <t>0.04921412467956543</t>
+          <t>0.049195826053619385</t>
         </is>
       </c>
       <c r="Z21" s="3" t="inlineStr">
         <is>
-          <t>-0.054457664489746094</t>
+          <t>-0.05447590351104736</t>
         </is>
       </c>
       <c r="AA21" s="3" t="inlineStr">
         <is>
-          <t>-0.05446678400039673</t>
+          <t>-0.05449157953262329</t>
         </is>
       </c>
       <c r="AB21" s="3" t="inlineStr">
         <is>
-          <t>1.602048397064209</t>
+          <t>1.6020491123199463</t>
         </is>
       </c>
       <c r="AC21" s="3" t="inlineStr">
         <is>
-          <t>-1.6028515100479126</t>
+          <t>-1.6028478145599365</t>
         </is>
       </c>
       <c r="AD21" s="3" t="inlineStr">
         <is>
-          <t>-1.6015112400054932</t>
+          <t>-1.6015090942382812</t>
         </is>
       </c>
       <c r="AE21" s="3" t="inlineStr">
         <is>
-          <t>1.6032164096832275</t>
+          <t>1.6032156944274902</t>
         </is>
       </c>
       <c r="AF21" s="3" t="inlineStr">
@@ -12623,17 +12623,17 @@
       </c>
       <c r="P22" s="3" t="inlineStr">
         <is>
-          <t>300.1788635253906</t>
+          <t>300.3526611328125</t>
         </is>
       </c>
       <c r="Q22" s="3" t="inlineStr">
         <is>
-          <t>-498.02227783203125</t>
+          <t>-497.8447570800781</t>
         </is>
       </c>
       <c r="R22" s="3" t="inlineStr">
         <is>
-          <t>138.97088623046875</t>
+          <t>138.97000122070312</t>
         </is>
       </c>
       <c r="S22" s="3" t="inlineStr">
@@ -12663,42 +12663,42 @@
       </c>
       <c r="X22" s="3" t="inlineStr">
         <is>
-          <t>0.04844599962234497</t>
+          <t>0.04844164848327637</t>
         </is>
       </c>
       <c r="Y22" s="3" t="inlineStr">
         <is>
-          <t>0.048409104347229004</t>
+          <t>0.04843348264694214</t>
         </is>
       </c>
       <c r="Z22" s="3" t="inlineStr">
         <is>
-          <t>-0.054585814476013184</t>
+          <t>-0.05458444356918335</t>
         </is>
       </c>
       <c r="AA22" s="3" t="inlineStr">
         <is>
-          <t>-0.05459696054458618</t>
+          <t>-0.054601430892944336</t>
         </is>
       </c>
       <c r="AB22" s="3" t="inlineStr">
         <is>
-          <t>1.6019036769866943</t>
+          <t>1.601881504058838</t>
         </is>
       </c>
       <c r="AC22" s="3" t="inlineStr">
         <is>
-          <t>-1.6026568412780762</t>
+          <t>-1.6026561260223389</t>
         </is>
       </c>
       <c r="AD22" s="3" t="inlineStr">
         <is>
-          <t>-1.6015424728393555</t>
+          <t>-1.6015632152557373</t>
         </is>
       </c>
       <c r="AE22" s="3" t="inlineStr">
         <is>
-          <t>1.6032593250274658</t>
+          <t>1.6032356023788452</t>
         </is>
       </c>
       <c r="AF22" s="3" t="inlineStr">
@@ -13215,17 +13215,17 @@
       </c>
       <c r="P23" s="3" t="inlineStr">
         <is>
-          <t>299.4065856933594</t>
+          <t>299.58038330078125</t>
         </is>
       </c>
       <c r="Q23" s="3" t="inlineStr">
         <is>
-          <t>-498.7107849121094</t>
+          <t>-498.5332336425781</t>
         </is>
       </c>
       <c r="R23" s="3" t="inlineStr">
         <is>
-          <t>138.97447204589844</t>
+          <t>138.9735870361328</t>
         </is>
       </c>
       <c r="S23" s="3" t="inlineStr">
@@ -13255,42 +13255,42 @@
       </c>
       <c r="X23" s="3" t="inlineStr">
         <is>
-          <t>0.049264371395111084</t>
+          <t>0.04928255081176758</t>
         </is>
       </c>
       <c r="Y23" s="3" t="inlineStr">
         <is>
-          <t>0.04925274848937988</t>
+          <t>0.049277663230895996</t>
         </is>
       </c>
       <c r="Z23" s="3" t="inlineStr">
         <is>
-          <t>-0.05445903539657593</t>
+          <t>-0.05443418025970459</t>
         </is>
       </c>
       <c r="AA23" s="3" t="inlineStr">
         <is>
-          <t>-0.05446535348892212</t>
+          <t>-0.054447174072265625</t>
         </is>
       </c>
       <c r="AB23" s="3" t="inlineStr">
         <is>
-          <t>1.6019588708877563</t>
+          <t>1.601956844329834</t>
         </is>
       </c>
       <c r="AC23" s="3" t="inlineStr">
         <is>
-          <t>-1.6027686595916748</t>
+          <t>-1.6027679443359375</t>
         </is>
       </c>
       <c r="AD23" s="3" t="inlineStr">
         <is>
-          <t>-1.6013816595077515</t>
+          <t>-1.6013826131820679</t>
         </is>
       </c>
       <c r="AE23" s="3" t="inlineStr">
         <is>
-          <t>1.6030875444412231</t>
+          <t>1.603083848953247</t>
         </is>
       </c>
       <c r="AF23" s="3" t="inlineStr">
@@ -13807,17 +13807,17 @@
       </c>
       <c r="P24" s="3" t="inlineStr">
         <is>
-          <t>300.2557678222656</t>
+          <t>300.4295654296875</t>
         </is>
       </c>
       <c r="Q24" s="3" t="inlineStr">
         <is>
-          <t>-497.9537353515625</t>
+          <t>-497.77618408203125</t>
         </is>
       </c>
       <c r="R24" s="3" t="inlineStr">
         <is>
-          <t>138.9705352783203</t>
+          <t>138.9696502685547</t>
         </is>
       </c>
       <c r="S24" s="3" t="inlineStr">
@@ -13847,42 +13847,42 @@
       </c>
       <c r="X24" s="3" t="inlineStr">
         <is>
-          <t>0.04836142063140869</t>
+          <t>0.04833662509918213</t>
         </is>
       </c>
       <c r="Y24" s="3" t="inlineStr">
         <is>
-          <t>0.048341453075408936</t>
+          <t>0.04832327365875244</t>
         </is>
       </c>
       <c r="Z24" s="3" t="inlineStr">
         <is>
-          <t>-0.05459034442901611</t>
+          <t>-0.05458557605743408</t>
         </is>
       </c>
       <c r="AA24" s="3" t="inlineStr">
         <is>
-          <t>-0.05457240343093872</t>
+          <t>-0.054597318172454834</t>
         </is>
       </c>
       <c r="AB24" s="3" t="inlineStr">
         <is>
-          <t>1.6017577648162842</t>
+          <t>1.601758599281311</t>
         </is>
       </c>
       <c r="AC24" s="3" t="inlineStr">
         <is>
-          <t>-1.6025214195251465</t>
+          <t>-1.6025177240371704</t>
         </is>
       </c>
       <c r="AD24" s="3" t="inlineStr">
         <is>
-          <t>-1.601433515548706</t>
+          <t>-1.6014115810394287</t>
         </is>
       </c>
       <c r="AE24" s="3" t="inlineStr">
         <is>
-          <t>1.603126883506775</t>
+          <t>1.6031261682510376</t>
         </is>
       </c>
       <c r="AF24" s="3" t="inlineStr">
@@ -14399,17 +14399,17 @@
       </c>
       <c r="P25" s="3" t="inlineStr">
         <is>
-          <t>299.3291015625</t>
+          <t>299.5028991699219</t>
         </is>
       </c>
       <c r="Q25" s="3" t="inlineStr">
         <is>
-          <t>-498.7798767089844</t>
+          <t>-498.602294921875</t>
         </is>
       </c>
       <c r="R25" s="3" t="inlineStr">
         <is>
-          <t>138.97482299804688</t>
+          <t>138.97393798828125</t>
         </is>
       </c>
       <c r="S25" s="3" t="inlineStr">
@@ -14439,42 +14439,42 @@
       </c>
       <c r="X25" s="3" t="inlineStr">
         <is>
-          <t>0.0493510365486145</t>
+          <t>0.04934960603713989</t>
         </is>
       </c>
       <c r="Y25" s="3" t="inlineStr">
         <is>
-          <t>0.049338340759277344</t>
+          <t>0.04934275150299072</t>
         </is>
       </c>
       <c r="Z25" s="3" t="inlineStr">
         <is>
-          <t>-0.054416537284851074</t>
+          <t>-0.054412126541137695</t>
         </is>
       </c>
       <c r="AA25" s="3" t="inlineStr">
         <is>
-          <t>-0.05442178249359131</t>
+          <t>-0.05444622039794922</t>
         </is>
       </c>
       <c r="AB25" s="3" t="inlineStr">
         <is>
-          <t>1.6018235683441162</t>
+          <t>1.601844310760498</t>
         </is>
       </c>
       <c r="AC25" s="3" t="inlineStr">
         <is>
-          <t>-1.6026458740234375</t>
+          <t>-1.6026220321655273</t>
         </is>
       </c>
       <c r="AD25" s="3" t="inlineStr">
         <is>
-          <t>-1.601255178451538</t>
+          <t>-1.6012330055236816</t>
         </is>
       </c>
       <c r="AE25" s="3" t="inlineStr">
         <is>
-          <t>1.6029558181762695</t>
+          <t>1.6029548645019531</t>
         </is>
       </c>
       <c r="AF25" s="3" t="inlineStr">
@@ -14991,17 +14991,17 @@
       </c>
       <c r="P26" s="3" t="inlineStr">
         <is>
-          <t>300.3326110839844</t>
+          <t>300.50640869140625</t>
         </is>
       </c>
       <c r="Q26" s="3" t="inlineStr">
         <is>
-          <t>-497.8852233886719</t>
+          <t>-497.70770263671875</t>
         </is>
       </c>
       <c r="R26" s="3" t="inlineStr">
         <is>
-          <t>138.97018432617188</t>
+          <t>138.96929931640625</t>
         </is>
       </c>
       <c r="S26" s="3" t="inlineStr">
@@ -15031,42 +15031,42 @@
       </c>
       <c r="X26" s="3" t="inlineStr">
         <is>
-          <t>0.04825347661972046</t>
+          <t>0.04824864864349365</t>
         </is>
       </c>
       <c r="Y26" s="3" t="inlineStr">
         <is>
-          <t>0.04823124408721924</t>
+          <t>0.048236072063446045</t>
         </is>
       </c>
       <c r="Z26" s="3" t="inlineStr">
         <is>
-          <t>-0.054591476917266846</t>
+          <t>-0.054589688777923584</t>
         </is>
       </c>
       <c r="AA26" s="3" t="inlineStr">
         <is>
-          <t>-0.054591357707977295</t>
+          <t>-0.0545961856842041</t>
         </is>
       </c>
       <c r="AB26" s="3" t="inlineStr">
         <is>
-          <t>1.6015918254852295</t>
+          <t>1.6015695333480835</t>
         </is>
       </c>
       <c r="AC26" s="3" t="inlineStr">
         <is>
-          <t>-1.6023828983306885</t>
+          <t>-1.6023592948913574</t>
         </is>
       </c>
       <c r="AD26" s="3" t="inlineStr">
         <is>
-          <t>-1.601281762123108</t>
+          <t>-1.6013026237487793</t>
         </is>
       </c>
       <c r="AE26" s="3" t="inlineStr">
         <is>
-          <t>1.6029975414276123</t>
+          <t>1.6029735803604126</t>
         </is>
       </c>
       <c r="AF26" s="3" t="inlineStr">
@@ -15583,17 +15583,17 @@
       </c>
       <c r="P27" s="3" t="inlineStr">
         <is>
-          <t>299.2515869140625</t>
+          <t>299.4253845214844</t>
         </is>
       </c>
       <c r="Q27" s="3" t="inlineStr">
         <is>
-          <t>-498.8489685058594</t>
+          <t>-498.6714172363281</t>
         </is>
       </c>
       <c r="R27" s="3" t="inlineStr">
         <is>
-          <t>138.97518920898438</t>
+          <t>138.97430419921875</t>
         </is>
       </c>
       <c r="S27" s="3" t="inlineStr">
@@ -15623,42 +15623,42 @@
       </c>
       <c r="X27" s="3" t="inlineStr">
         <is>
-          <t>0.049418509006500244</t>
+          <t>0.04941403865814209</t>
         </is>
       </c>
       <c r="Y27" s="3" t="inlineStr">
         <is>
-          <t>0.04940301179885864</t>
+          <t>0.04942750930786133</t>
         </is>
       </c>
       <c r="Z27" s="3" t="inlineStr">
         <is>
-          <t>-0.05439192056655884</t>
+          <t>-0.05436736345291138</t>
         </is>
       </c>
       <c r="AA27" s="3" t="inlineStr">
         <is>
-          <t>-0.05440032482147217</t>
+          <t>-0.0544048547744751</t>
         </is>
       </c>
       <c r="AB27" s="3" t="inlineStr">
         <is>
-          <t>1.6017110347747803</t>
+          <t>1.6016888618469238</t>
         </is>
       </c>
       <c r="AC27" s="3" t="inlineStr">
         <is>
-          <t>-1.6024999618530273</t>
+          <t>-1.60249924659729</t>
         </is>
       </c>
       <c r="AD27" s="3" t="inlineStr">
         <is>
-          <t>-1.6010626554489136</t>
+          <t>-1.6010634899139404</t>
         </is>
       </c>
       <c r="AE27" s="3" t="inlineStr">
         <is>
-          <t>1.6028039455413818</t>
+          <t>1.6027801036834717</t>
         </is>
       </c>
       <c r="AF27" s="3" t="inlineStr">
@@ -16175,17 +16175,17 @@
       </c>
       <c r="P28" s="3" t="inlineStr">
         <is>
-          <t>300.40936279296875</t>
+          <t>300.5831604003906</t>
         </is>
       </c>
       <c r="Q28" s="3" t="inlineStr">
         <is>
-          <t>-497.8168029785156</t>
+          <t>-497.6392517089844</t>
         </is>
       </c>
       <c r="R28" s="3" t="inlineStr">
         <is>
-          <t>138.96981811523438</t>
+          <t>138.96893310546875</t>
         </is>
       </c>
       <c r="S28" s="3" t="inlineStr">
@@ -16215,42 +16215,42 @@
       </c>
       <c r="X28" s="3" t="inlineStr">
         <is>
-          <t>0.048188209533691406</t>
+          <t>0.04816335439682007</t>
         </is>
       </c>
       <c r="Y28" s="3" t="inlineStr">
         <is>
-          <t>0.04814726114273071</t>
+          <t>0.04815208911895752</t>
         </is>
       </c>
       <c r="Z28" s="3" t="inlineStr">
         <is>
-          <t>-0.054572224617004395</t>
+          <t>-0.05458742380142212</t>
         </is>
       </c>
       <c r="AA28" s="3" t="inlineStr">
         <is>
-          <t>-0.054570555686950684</t>
+          <t>-0.05459541082382202</t>
         </is>
       </c>
       <c r="AB28" s="3" t="inlineStr">
         <is>
-          <t>1.601422905921936</t>
+          <t>1.6014236211776733</t>
         </is>
       </c>
       <c r="AC28" s="3" t="inlineStr">
         <is>
-          <t>-1.6021814346313477</t>
+          <t>-1.6021575927734375</t>
         </is>
       </c>
       <c r="AD28" s="3" t="inlineStr">
         <is>
-          <t>-1.6011528968811035</t>
+          <t>-1.6011077165603638</t>
         </is>
       </c>
       <c r="AE28" s="3" t="inlineStr">
         <is>
-          <t>1.6028218269348145</t>
+          <t>1.602820873260498</t>
         </is>
       </c>
       <c r="AF28" s="3" t="inlineStr">
@@ -16767,17 +16767,17 @@
       </c>
       <c r="P29" s="3" t="inlineStr">
         <is>
-          <t>299.1740417480469</t>
+          <t>299.34783935546875</t>
         </is>
       </c>
       <c r="Q29" s="3" t="inlineStr">
         <is>
-          <t>-498.9181213378906</t>
+          <t>-498.74053955078125</t>
         </is>
       </c>
       <c r="R29" s="3" t="inlineStr">
         <is>
-          <t>138.97555541992188</t>
+          <t>138.97467041015625</t>
         </is>
       </c>
       <c r="S29" s="3" t="inlineStr">
@@ -16807,42 +16807,42 @@
       </c>
       <c r="X29" s="3" t="inlineStr">
         <is>
-          <t>0.04950296878814697</t>
+          <t>0.04947805404663086</t>
         </is>
       </c>
       <c r="Y29" s="3" t="inlineStr">
         <is>
-          <t>0.04949080944061279</t>
+          <t>0.0494956374168396</t>
         </is>
       </c>
       <c r="Z29" s="3" t="inlineStr">
         <is>
-          <t>-0.05436718463897705</t>
+          <t>-0.054362356662750244</t>
         </is>
       </c>
       <c r="AA29" s="3" t="inlineStr">
         <is>
-          <t>-0.054361939430236816</t>
+          <t>-0.054363787174224854</t>
         </is>
       </c>
       <c r="AB29" s="3" t="inlineStr">
         <is>
-          <t>1.6015325784683228</t>
+          <t>1.60153329372406</t>
         </is>
       </c>
       <c r="AC29" s="3" t="inlineStr">
         <is>
-          <t>-1.6023340225219727</t>
+          <t>-1.6023101806640625</t>
         </is>
       </c>
       <c r="AD29" s="3" t="inlineStr">
         <is>
-          <t>-1.600870132446289</t>
+          <t>-1.600847840309143</t>
         </is>
       </c>
       <c r="AE29" s="3" t="inlineStr">
         <is>
-          <t>1.602586030960083</t>
+          <t>1.6026052236557007</t>
         </is>
       </c>
       <c r="AF29" s="3" t="inlineStr">
@@ -17359,17 +17359,17 @@
       </c>
       <c r="P30" s="3" t="inlineStr">
         <is>
-          <t>300.4860534667969</t>
+          <t>300.65985107421875</t>
         </is>
       </c>
       <c r="Q30" s="3" t="inlineStr">
         <is>
-          <t>-497.7484130859375</t>
+          <t>-497.5708923339844</t>
         </is>
       </c>
       <c r="R30" s="3" t="inlineStr">
         <is>
-          <t>138.96946716308594</t>
+          <t>138.9685821533203</t>
         </is>
       </c>
       <c r="S30" s="3" t="inlineStr">
@@ -17399,42 +17399,42 @@
       </c>
       <c r="X30" s="3" t="inlineStr">
         <is>
-          <t>0.04805713891983032</t>
+          <t>0.04805272817611694</t>
         </is>
       </c>
       <c r="Y30" s="3" t="inlineStr">
         <is>
-          <t>0.04804307222366333</t>
+          <t>0.04806751012802124</t>
         </is>
       </c>
       <c r="Z30" s="3" t="inlineStr">
         <is>
-          <t>-0.05459040403366089</t>
+          <t>-0.054566025733947754</t>
         </is>
       </c>
       <c r="AA30" s="3" t="inlineStr">
         <is>
-          <t>-0.05456948280334473</t>
+          <t>-0.054573893547058105</t>
         </is>
       </c>
       <c r="AB30" s="3" t="inlineStr">
         <is>
-          <t>1.6012370586395264</t>
+          <t>1.6012146472930908</t>
         </is>
       </c>
       <c r="AC30" s="3" t="inlineStr">
         <is>
-          <t>-1.6019569635391235</t>
+          <t>-1.6019561290740967</t>
         </is>
       </c>
       <c r="AD30" s="3" t="inlineStr">
         <is>
-          <t>-1.6009351015090942</t>
+          <t>-1.600935935974121</t>
         </is>
       </c>
       <c r="AE30" s="3" t="inlineStr">
         <is>
-          <t>1.6026694774627686</t>
+          <t>1.6026455163955688</t>
         </is>
       </c>
       <c r="AF30" s="3" t="inlineStr">
@@ -17951,17 +17951,17 @@
       </c>
       <c r="P31" s="3" t="inlineStr">
         <is>
-          <t>299.0964660644531</t>
+          <t>299.270263671875</t>
         </is>
       </c>
       <c r="Q31" s="3" t="inlineStr">
         <is>
-          <t>-498.9872741699219</t>
+          <t>-498.8097229003906</t>
         </is>
       </c>
       <c r="R31" s="3" t="inlineStr">
         <is>
-          <t>138.9759063720703</t>
+          <t>138.9750213623047</t>
         </is>
       </c>
       <c r="S31" s="3" t="inlineStr">
@@ -17991,42 +17991,42 @@
       </c>
       <c r="X31" s="3" t="inlineStr">
         <is>
-          <t>0.0495639443397522</t>
+          <t>0.04958212375640869</t>
         </is>
       </c>
       <c r="Y31" s="3" t="inlineStr">
         <is>
-          <t>0.04953891038894653</t>
+          <t>0.049563825130462646</t>
         </is>
       </c>
       <c r="Z31" s="3" t="inlineStr">
         <is>
-          <t>-0.054319024085998535</t>
+          <t>-0.05429422855377197</t>
         </is>
       </c>
       <c r="AA31" s="3" t="inlineStr">
         <is>
-          <t>-0.054343998432159424</t>
+          <t>-0.05430573225021362</t>
         </is>
       </c>
       <c r="AB31" s="3" t="inlineStr">
         <is>
-          <t>1.6013340950012207</t>
+          <t>1.6013317108154297</t>
         </is>
       </c>
       <c r="AC31" s="3" t="inlineStr">
         <is>
-          <t>-1.6021220684051514</t>
+          <t>-1.602121353149414</t>
         </is>
       </c>
       <c r="AD31" s="3" t="inlineStr">
         <is>
-          <t>-1.6006574630737305</t>
+          <t>-1.6006581783294678</t>
         </is>
       </c>
       <c r="AE31" s="3" t="inlineStr">
         <is>
-          <t>1.602391242980957</t>
+          <t>1.6023643016815186</t>
         </is>
       </c>
       <c r="AF31" s="3" t="inlineStr">
@@ -18543,17 +18543,17 @@
       </c>
       <c r="P32" s="3" t="inlineStr">
         <is>
-          <t>300.56268310546875</t>
+          <t>300.7364807128906</t>
         </is>
       </c>
       <c r="Q32" s="3" t="inlineStr">
         <is>
-          <t>-497.68011474609375</t>
+          <t>-497.5025939941406</t>
         </is>
       </c>
       <c r="R32" s="3" t="inlineStr">
         <is>
-          <t>138.9691162109375</t>
+          <t>138.96823120117188</t>
         </is>
       </c>
       <c r="S32" s="3" t="inlineStr">
@@ -18583,42 +18583,42 @@
       </c>
       <c r="X32" s="3" t="inlineStr">
         <is>
-          <t>0.04794353246688843</t>
+          <t>0.04796183109283447</t>
         </is>
       </c>
       <c r="Y32" s="3" t="inlineStr">
         <is>
-          <t>0.04793834686279297</t>
+          <t>0.047943174839019775</t>
         </is>
       </c>
       <c r="Z32" s="3" t="inlineStr">
         <is>
-          <t>-0.05458897352218628</t>
+          <t>-0.05456411838531494</t>
         </is>
       </c>
       <c r="AA32" s="3" t="inlineStr">
         <is>
-          <t>-0.05459392070770264</t>
+          <t>-0.05459874868392944</t>
         </is>
       </c>
       <c r="AB32" s="3" t="inlineStr">
         <is>
-          <t>1.600984811782837</t>
+          <t>1.600982666015625</t>
         </is>
       </c>
       <c r="AC32" s="3" t="inlineStr">
         <is>
-          <t>-1.6017322540283203</t>
+          <t>-1.6017085313796997</t>
         </is>
       </c>
       <c r="AD32" s="3" t="inlineStr">
         <is>
-          <t>-1.6007400751113892</t>
+          <t>-1.600740909576416</t>
         </is>
       </c>
       <c r="AE32" s="3" t="inlineStr">
         <is>
-          <t>1.6024537086486816</t>
+          <t>1.6024298667907715</t>
         </is>
       </c>
       <c r="AF32" s="3" t="inlineStr">
@@ -19135,17 +19135,17 @@
       </c>
       <c r="P33" s="3" t="inlineStr">
         <is>
-          <t>299.01885986328125</t>
+          <t>299.19268798828125</t>
         </is>
       </c>
       <c r="Q33" s="3" t="inlineStr">
         <is>
-          <t>-499.05645751953125</t>
+          <t>-498.87890625</t>
         </is>
       </c>
       <c r="R33" s="3" t="inlineStr">
         <is>
-          <t>138.9762725830078</t>
+          <t>138.9753875732422</t>
         </is>
       </c>
       <c r="S33" s="3" t="inlineStr">
@@ -19175,42 +19175,42 @@
       </c>
       <c r="X33" s="3" t="inlineStr">
         <is>
-          <t>0.049625396728515625</t>
+          <t>0.04964059591293335</t>
         </is>
       </c>
       <c r="Y33" s="3" t="inlineStr">
         <is>
-          <t>0.04962962865829468</t>
+          <t>0.049631476402282715</t>
         </is>
       </c>
       <c r="Z33" s="3" t="inlineStr">
         <is>
-          <t>-0.054291367530822754</t>
+          <t>-0.05428957939147949</t>
         </is>
       </c>
       <c r="AA33" s="3" t="inlineStr">
         <is>
-          <t>-0.054285526275634766</t>
+          <t>-0.05431336164474487</t>
         </is>
       </c>
       <c r="AB33" s="3" t="inlineStr">
         <is>
-          <t>1.601135492324829</t>
+          <t>1.6010901927947998</t>
         </is>
       </c>
       <c r="AC33" s="3" t="inlineStr">
         <is>
-          <t>-1.6019132137298584</t>
+          <t>-1.6019322872161865</t>
         </is>
       </c>
       <c r="AD33" s="3" t="inlineStr">
         <is>
-          <t>-1.600421667098999</t>
+          <t>-1.60044264793396</t>
         </is>
       </c>
       <c r="AE33" s="3" t="inlineStr">
         <is>
-          <t>1.6021502017974854</t>
+          <t>1.6021063327789307</t>
         </is>
       </c>
       <c r="AF33" s="3" t="inlineStr">
@@ -19727,17 +19727,17 @@
       </c>
       <c r="P34" s="3" t="inlineStr">
         <is>
-          <t>300.63922119140625</t>
+          <t>300.8130187988281</t>
         </is>
       </c>
       <c r="Q34" s="3" t="inlineStr">
         <is>
-          <t>-497.6119079589844</t>
+          <t>-497.43438720703125</t>
         </is>
       </c>
       <c r="R34" s="3" t="inlineStr">
         <is>
-          <t>138.96875</t>
+          <t>138.96786499023438</t>
         </is>
       </c>
       <c r="S34" s="3" t="inlineStr">
@@ -19767,42 +19767,42 @@
       </c>
       <c r="X34" s="3" t="inlineStr">
         <is>
-          <t>0.047849178314208984</t>
+          <t>0.04786747694015503</t>
         </is>
       </c>
       <c r="Y34" s="3" t="inlineStr">
         <is>
-          <t>0.047857463359832764</t>
+          <t>0.04783928394317627</t>
         </is>
       </c>
       <c r="Z34" s="3" t="inlineStr">
         <is>
-          <t>-0.05456364154815674</t>
+          <t>-0.05455893278121948</t>
         </is>
       </c>
       <c r="AA34" s="3" t="inlineStr">
         <is>
-          <t>-0.054579198360443115</t>
+          <t>-0.05456089973449707</t>
         </is>
       </c>
       <c r="AB34" s="3" t="inlineStr">
         <is>
-          <t>1.6007099151611328</t>
+          <t>1.6007075309753418</t>
         </is>
       </c>
       <c r="AC34" s="3" t="inlineStr">
         <is>
-          <t>-1.6014878749847412</t>
+          <t>-1.6014840602874756</t>
         </is>
       </c>
       <c r="AD34" s="3" t="inlineStr">
         <is>
-          <t>-1.600525140762329</t>
+          <t>-1.6005029678344727</t>
         </is>
       </c>
       <c r="AE34" s="3" t="inlineStr">
         <is>
-          <t>1.6021920442581177</t>
+          <t>1.602188229560852</t>
         </is>
       </c>
       <c r="AF34" s="3" t="inlineStr">
@@ -20319,17 +20319,17 @@
       </c>
       <c r="P35" s="3" t="inlineStr">
         <is>
-          <t>298.9412536621094</t>
+          <t>299.11505126953125</t>
         </is>
       </c>
       <c r="Q35" s="3" t="inlineStr">
         <is>
-          <t>-499.12567138671875</t>
+          <t>-498.9480895996094</t>
         </is>
       </c>
       <c r="R35" s="3" t="inlineStr">
         <is>
-          <t>138.97662353515625</t>
+          <t>138.97573852539062</t>
         </is>
       </c>
       <c r="S35" s="3" t="inlineStr">
@@ -20359,42 +20359,42 @@
       </c>
       <c r="X35" s="3" t="inlineStr">
         <is>
-          <t>0.049703001976013184</t>
+          <t>0.04967862367630005</t>
         </is>
       </c>
       <c r="Y35" s="3" t="inlineStr">
         <is>
-          <t>0.04967820644378662</t>
+          <t>0.049682557582855225</t>
         </is>
       </c>
       <c r="Z35" s="3" t="inlineStr">
         <is>
-          <t>-0.05425983667373657</t>
+          <t>-0.054255545139312744</t>
         </is>
       </c>
       <c r="AA35" s="3" t="inlineStr">
         <is>
-          <t>-0.05427396297454834</t>
+          <t>-0.05425524711608887</t>
         </is>
       </c>
       <c r="AB35" s="3" t="inlineStr">
         <is>
-          <t>1.6008708477020264</t>
+          <t>1.6008715629577637</t>
         </is>
       </c>
       <c r="AC35" s="3" t="inlineStr">
         <is>
-          <t>-1.601701021194458</t>
+          <t>-1.601677417755127</t>
         </is>
       </c>
       <c r="AD35" s="3" t="inlineStr">
         <is>
-          <t>-1.6001430749893188</t>
+          <t>-1.600121021270752</t>
         </is>
       </c>
       <c r="AE35" s="3" t="inlineStr">
         <is>
-          <t>1.6018691062927246</t>
+          <t>1.6018654108047485</t>
         </is>
       </c>
       <c r="AF35" s="3" t="inlineStr">
@@ -20911,17 +20911,17 @@
       </c>
       <c r="P36" s="3" t="inlineStr">
         <is>
-          <t>300.7156677246094</t>
+          <t>300.88946533203125</t>
         </is>
       </c>
       <c r="Q36" s="3" t="inlineStr">
         <is>
-          <t>-497.54376220703125</t>
+          <t>-497.3662414550781</t>
         </is>
       </c>
       <c r="R36" s="3" t="inlineStr">
         <is>
-          <t>138.96839904785156</t>
+          <t>138.96751403808594</t>
         </is>
       </c>
       <c r="S36" s="3" t="inlineStr">
@@ -20951,42 +20951,42 @@
       </c>
       <c r="X36" s="3" t="inlineStr">
         <is>
-          <t>0.04773533344268799</t>
+          <t>0.04775357246398926</t>
         </is>
       </c>
       <c r="Y36" s="3" t="inlineStr">
         <is>
-          <t>0.04773610830307007</t>
+          <t>0.04773789644241333</t>
         </is>
       </c>
       <c r="Z36" s="3" t="inlineStr">
         <is>
-          <t>-0.054535865783691406</t>
+          <t>-0.054554104804992676</t>
         </is>
       </c>
       <c r="AA36" s="3" t="inlineStr">
         <is>
-          <t>-0.05456387996673584</t>
+          <t>-0.054545700550079346</t>
         </is>
       </c>
       <c r="AB36" s="3" t="inlineStr">
         <is>
-          <t>1.600457787513733</t>
+          <t>1.6004555225372314</t>
         </is>
       </c>
       <c r="AC36" s="3" t="inlineStr">
         <is>
-          <t>-1.6011972427368164</t>
+          <t>-1.601216435432434</t>
         </is>
       </c>
       <c r="AD36" s="3" t="inlineStr">
         <is>
-          <t>-1.6002671718597412</t>
+          <t>-1.6002650260925293</t>
         </is>
       </c>
       <c r="AE36" s="3" t="inlineStr">
         <is>
-          <t>1.6019303798675537</t>
+          <t>1.601926565170288</t>
         </is>
       </c>
       <c r="AF36" s="3" t="inlineStr">
@@ -21503,17 +21503,17 @@
       </c>
       <c r="P37" s="3" t="inlineStr">
         <is>
-          <t>298.8636169433594</t>
+          <t>299.03741455078125</t>
         </is>
       </c>
       <c r="Q37" s="3" t="inlineStr">
         <is>
-          <t>-499.19488525390625</t>
+          <t>-499.017333984375</t>
         </is>
       </c>
       <c r="R37" s="3" t="inlineStr">
         <is>
-          <t>138.97698974609375</t>
+          <t>138.97610473632812</t>
         </is>
       </c>
       <c r="S37" s="3" t="inlineStr">
@@ -21543,42 +21543,42 @@
       </c>
       <c r="X37" s="3" t="inlineStr">
         <is>
-          <t>0.049738526344299316</t>
+          <t>0.04977679252624512</t>
         </is>
       </c>
       <c r="Y37" s="3" t="inlineStr">
         <is>
-          <t>0.0497317910194397</t>
+          <t>0.04975658655166626</t>
         </is>
       </c>
       <c r="Z37" s="3" t="inlineStr">
         <is>
-          <t>-0.05422931909561157</t>
+          <t>-0.05420452356338501</t>
         </is>
       </c>
       <c r="AA37" s="3" t="inlineStr">
         <is>
-          <t>-0.05423849821090698</t>
+          <t>-0.05420023202896118</t>
         </is>
       </c>
       <c r="AB37" s="3" t="inlineStr">
         <is>
-          <t>1.600609302520752</t>
+          <t>1.6005840301513672</t>
         </is>
       </c>
       <c r="AC37" s="3" t="inlineStr">
         <is>
-          <t>-1.6014031171798706</t>
+          <t>-1.6014022827148438</t>
         </is>
       </c>
       <c r="AD37" s="3" t="inlineStr">
         <is>
-          <t>-1.5998643636703491</t>
+          <t>-1.599865198135376</t>
         </is>
       </c>
       <c r="AE37" s="3" t="inlineStr">
         <is>
-          <t>1.6016082763671875</t>
+          <t>1.601581335067749</t>
         </is>
       </c>
       <c r="AF37" s="3" t="inlineStr">
@@ -22095,17 +22095,17 @@
       </c>
       <c r="P38" s="3" t="inlineStr">
         <is>
-          <t>300.7920227050781</t>
+          <t>300.9658203125</t>
         </is>
       </c>
       <c r="Q38" s="3" t="inlineStr">
         <is>
-          <t>-497.4756774902344</t>
+          <t>-497.29815673828125</t>
         </is>
       </c>
       <c r="R38" s="3" t="inlineStr">
         <is>
-          <t>138.96804809570312</t>
+          <t>138.9671630859375</t>
         </is>
       </c>
       <c r="S38" s="3" t="inlineStr">
@@ -22135,42 +22135,42 @@
       </c>
       <c r="X38" s="3" t="inlineStr">
         <is>
-          <t>0.04764169454574585</t>
+          <t>0.04763692617416382</t>
         </is>
       </c>
       <c r="Y38" s="3" t="inlineStr">
         <is>
-          <t>0.0476374626159668</t>
+          <t>0.04761922359466553</t>
         </is>
       </c>
       <c r="Z38" s="3" t="inlineStr">
         <is>
-          <t>-0.05454838275909424</t>
+          <t>-0.05454665422439575</t>
         </is>
       </c>
       <c r="AA38" s="3" t="inlineStr">
         <is>
-          <t>-0.05456840991973877</t>
+          <t>-0.054550230503082275</t>
         </is>
       </c>
       <c r="AB38" s="3" t="inlineStr">
         <is>
-          <t>1.6001826524734497</t>
+          <t>1.6001603603363037</t>
         </is>
       </c>
       <c r="AC38" s="3" t="inlineStr">
         <is>
-          <t>-1.600886583328247</t>
+          <t>-1.6008827686309814</t>
         </is>
       </c>
       <c r="AD38" s="3" t="inlineStr">
         <is>
-          <t>-1.5999631881713867</t>
+          <t>-1.5999839305877686</t>
         </is>
       </c>
       <c r="AE38" s="3" t="inlineStr">
         <is>
-          <t>1.6016918420791626</t>
+          <t>1.6016879081726074</t>
         </is>
       </c>
       <c r="AF38" s="3" t="inlineStr">
@@ -22687,17 +22687,17 @@
       </c>
       <c r="P39" s="3" t="inlineStr">
         <is>
-          <t>298.78594970703125</t>
+          <t>298.95977783203125</t>
         </is>
       </c>
       <c r="Q39" s="3" t="inlineStr">
         <is>
-          <t>-499.2641296386719</t>
+          <t>-499.0865478515625</t>
         </is>
       </c>
       <c r="R39" s="3" t="inlineStr">
         <is>
-          <t>138.97735595703125</t>
+          <t>138.97647094726562</t>
         </is>
       </c>
       <c r="S39" s="3" t="inlineStr">
@@ -22727,42 +22727,42 @@
       </c>
       <c r="X39" s="3" t="inlineStr">
         <is>
-          <t>0.049816906452178955</t>
+          <t>0.049812138080596924</t>
         </is>
       </c>
       <c r="Y39" s="3" t="inlineStr">
         <is>
-          <t>0.04980558156967163</t>
+          <t>0.049787282943725586</t>
         </is>
       </c>
       <c r="Z39" s="3" t="inlineStr">
         <is>
-          <t>-0.054172515869140625</t>
+          <t>-0.05417078733444214</t>
         </is>
       </c>
       <c r="AA39" s="3" t="inlineStr">
         <is>
-          <t>-0.05418616533279419</t>
+          <t>-0.05419081449508667</t>
         </is>
       </c>
       <c r="AB39" s="3" t="inlineStr">
         <is>
-          <t>1.6003445386886597</t>
+          <t>1.6003223657608032</t>
         </is>
       </c>
       <c r="AC39" s="3" t="inlineStr">
         <is>
-          <t>-1.6011279821395874</t>
+          <t>-1.6011242866516113</t>
         </is>
       </c>
       <c r="AD39" s="3" t="inlineStr">
         <is>
-          <t>-1.599522590637207</t>
+          <t>-1.5995434522628784</t>
         </is>
       </c>
       <c r="AE39" s="3" t="inlineStr">
         <is>
-          <t>1.6012811660766602</t>
+          <t>1.60125732421875</t>
         </is>
       </c>
       <c r="AF39" s="3" t="inlineStr">
@@ -23279,17 +23279,17 @@
       </c>
       <c r="P40" s="3" t="inlineStr">
         <is>
-          <t>300.8682861328125</t>
+          <t>301.0420837402344</t>
         </is>
       </c>
       <c r="Q40" s="3" t="inlineStr">
         <is>
-          <t>-497.4076843261719</t>
+          <t>-497.23016357421875</t>
         </is>
       </c>
       <c r="R40" s="3" t="inlineStr">
         <is>
-          <t>138.9676971435547</t>
+          <t>138.96681213378906</t>
         </is>
       </c>
       <c r="S40" s="3" t="inlineStr">
@@ -23319,42 +23319,42 @@
       </c>
       <c r="X40" s="3" t="inlineStr">
         <is>
-          <t>0.04754483699798584</t>
+          <t>0.047540128231048584</t>
         </is>
       </c>
       <c r="Y40" s="3" t="inlineStr">
         <is>
-          <t>0.047519028186798096</t>
+          <t>0.04752379655838013</t>
         </is>
       </c>
       <c r="Z40" s="3" t="inlineStr">
         <is>
-          <t>-0.05451768636703491</t>
+          <t>-0.054535865783691406</t>
         </is>
       </c>
       <c r="AA40" s="3" t="inlineStr">
         <is>
-          <t>-0.05453312397003174</t>
+          <t>-0.054537951946258545</t>
         </is>
       </c>
       <c r="AB40" s="3" t="inlineStr">
         <is>
-          <t>1.5998644828796387</t>
+          <t>1.5998423099517822</t>
         </is>
       </c>
       <c r="AC40" s="3" t="inlineStr">
         <is>
-          <t>-1.6005529165267944</t>
+          <t>-1.6005290746688843</t>
         </is>
       </c>
       <c r="AD40" s="3" t="inlineStr">
         <is>
-          <t>-1.5996620655059814</t>
+          <t>-1.5996599197387695</t>
         </is>
       </c>
       <c r="AE40" s="3" t="inlineStr">
         <is>
-          <t>1.6014070510864258</t>
+          <t>1.6013832092285156</t>
         </is>
       </c>
       <c r="AF40" s="3" t="inlineStr">
@@ -23871,17 +23871,17 @@
       </c>
       <c r="P41" s="3" t="inlineStr">
         <is>
-          <t>298.7082824707031</t>
+          <t>298.8821105957031</t>
         </is>
       </c>
       <c r="Q41" s="3" t="inlineStr">
         <is>
-          <t>-499.3333740234375</t>
+          <t>-499.1557922363281</t>
         </is>
       </c>
       <c r="R41" s="3" t="inlineStr">
         <is>
-          <t>138.97772216796875</t>
+          <t>138.97683715820312</t>
         </is>
       </c>
       <c r="S41" s="3" t="inlineStr">
@@ -23911,42 +23911,42 @@
       </c>
       <c r="X41" s="3" t="inlineStr">
         <is>
-          <t>0.04986929893493652</t>
+          <t>0.04986464977264404</t>
         </is>
       </c>
       <c r="Y41" s="3" t="inlineStr">
         <is>
-          <t>0.04986226558685303</t>
+          <t>0.049863994121551514</t>
         </is>
       </c>
       <c r="Z41" s="3" t="inlineStr">
         <is>
-          <t>-0.05413883924484253</t>
+          <t>-0.05415719747543335</t>
         </is>
       </c>
       <c r="AA41" s="3" t="inlineStr">
         <is>
-          <t>-0.05413365364074707</t>
+          <t>-0.05415838956832886</t>
         </is>
       </c>
       <c r="AB41" s="3" t="inlineStr">
         <is>
-          <t>1.6000168323516846</t>
+          <t>1.5999946594238281</t>
         </is>
       </c>
       <c r="AC41" s="3" t="inlineStr">
         <is>
-          <t>-1.600786805152893</t>
+          <t>-1.6008062362670898</t>
         </is>
       </c>
       <c r="AD41" s="3" t="inlineStr">
         <is>
-          <t>-1.59920072555542</t>
+          <t>-1.599198579788208</t>
         </is>
       </c>
       <c r="AE41" s="3" t="inlineStr">
         <is>
-          <t>1.6009540557861328</t>
+          <t>1.6009533405303955</t>
         </is>
       </c>
       <c r="AF41" s="3" t="inlineStr">
@@ -24463,17 +24463,17 @@
       </c>
       <c r="P42" s="3" t="inlineStr">
         <is>
-          <t>300.9444885253906</t>
+          <t>301.1182861328125</t>
         </is>
       </c>
       <c r="Q42" s="3" t="inlineStr">
         <is>
-          <t>-497.33978271484375</t>
+          <t>-497.1622619628906</t>
         </is>
       </c>
       <c r="R42" s="3" t="inlineStr">
         <is>
-          <t>138.96734619140625</t>
+          <t>138.96644592285156</t>
         </is>
       </c>
       <c r="S42" s="3" t="inlineStr">
@@ -24503,42 +24503,42 @@
       </c>
       <c r="X42" s="3" t="inlineStr">
         <is>
-          <t>0.04742187261581421</t>
+          <t>0.047416746616363525</t>
         </is>
       </c>
       <c r="Y42" s="3" t="inlineStr">
         <is>
-          <t>0.04740077257156372</t>
+          <t>0.04740583896636963</t>
         </is>
       </c>
       <c r="Z42" s="3" t="inlineStr">
         <is>
-          <t>-0.054529786109924316</t>
+          <t>-0.05452471971511841</t>
         </is>
       </c>
       <c r="AA42" s="3" t="inlineStr">
         <is>
-          <t>-0.05452394485473633</t>
+          <t>-0.05452907085418701</t>
         </is>
       </c>
       <c r="AB42" s="3" t="inlineStr">
         <is>
-          <t>1.5994832515716553</t>
+          <t>1.5994610786437988</t>
         </is>
       </c>
       <c r="AC42" s="3" t="inlineStr">
         <is>
-          <t>-1.6002192497253418</t>
+          <t>-1.6001954078674316</t>
         </is>
       </c>
       <c r="AD42" s="3" t="inlineStr">
         <is>
-          <t>-1.599358081817627</t>
+          <t>-1.5993359088897705</t>
         </is>
       </c>
       <c r="AE42" s="3" t="inlineStr">
         <is>
-          <t>1.6010594367980957</t>
+          <t>1.601035475730896</t>
         </is>
       </c>
       <c r="AF42" s="3" t="inlineStr">

</xml_diff>